<commit_message>
feat: color organizers in attendance list
</commit_message>
<xml_diff>
--- a/backend/xlsx_export/fixtures/attendance_list_template.xlsx
+++ b/backend/xlsx_export/fixtures/attendance_list_template.xlsx
@@ -214,7 +214,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -313,9 +313,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>336960</xdr:colOff>
+      <xdr:colOff>336600</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>144720</xdr:rowOff>
+      <xdr:rowOff>144360</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -329,7 +329,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="6175440" y="68040"/>
-          <a:ext cx="4632120" cy="1508040"/>
+          <a:ext cx="4631760" cy="1507680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -352,7 +352,7 @@
   <dimension ref="A1:H1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -427,7 +427,7 @@
       <c r="G5" s="2"/>
       <c r="H5" s="4"/>
     </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="19.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="2"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>

</xml_diff>